<commit_message>
update: new restrictions day/night/waking hours
</commit_message>
<xml_diff>
--- a/data/departments.xlsx
+++ b/data/departments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/birth_shotspotter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE331B1-369B-0C44-A354-E72714E6DD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AD0ABC-AD8C-FD47-9396-5A4471421BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{B476D8ED-B21E-A042-8580-B1D513862373}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C36"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update: append demos to addresses
</commit_message>
<xml_diff>
--- a/data/departments.xlsx
+++ b/data/departments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/birth_shotspotter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ECF3B5-3E21-E74C-8781-F8266A1B4D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1881C44-EE9D-3447-81A3-05D99BED3772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{B476D8ED-B21E-A042-8580-B1D513862373}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>city</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Final Cities working with</t>
+  </si>
+  <si>
+    <t>change in coverage in Sept 2019. Additional .2 sq miles</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92CB3F4-5A36-0F44-B549-82B3D687B3E8}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,6 +921,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>2008</v>
+      </c>
+      <c r="C36">
+        <v>2019</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: waking hours vs working hours
</commit_message>
<xml_diff>
--- a/data/departments.xlsx
+++ b/data/departments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/birth_shotspotter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1881C44-EE9D-3447-81A3-05D99BED3772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC73780-5C5E-AE4C-B86E-AA4B77BF87B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{B476D8ED-B21E-A042-8580-B1D513862373}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="16360" windowHeight="21600" xr2:uid="{B476D8ED-B21E-A042-8580-B1D513862373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>city</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>change in coverage in Sept 2019. Additional .2 sq miles</t>
+  </si>
+  <si>
+    <t>Oakland 1</t>
+  </si>
+  <si>
+    <t>Oakland 2</t>
   </si>
 </sst>
 </file>
@@ -197,10 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -259,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -365,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92CB3F4-5A36-0F44-B549-82B3D687B3E8}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,6 +945,118 @@
         <v>37</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43160</v>
+      </c>
+      <c r="C39" s="3">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3">
+        <v>39630</v>
+      </c>
+      <c r="C40" s="3">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3">
+        <v>42186</v>
+      </c>
+      <c r="C41" s="3">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3">
+        <v>39448</v>
+      </c>
+      <c r="C42" s="3">
+        <v>40483</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3">
+        <v>40756</v>
+      </c>
+      <c r="C43" s="3">
+        <v>41518</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="3">
+        <v>39904</v>
+      </c>
+      <c r="C44" s="3">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="3">
+        <v>42736</v>
+      </c>
+      <c r="C45" s="3">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="3">
+        <v>42370</v>
+      </c>
+      <c r="C46" s="3">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="3">
+        <v>41456</v>
+      </c>
+      <c r="C47" s="3">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3">
+        <v>41487</v>
+      </c>
+      <c r="C48" s="3">
+        <v>43313</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>